<commit_message>
Major change of code base (started)
</commit_message>
<xml_diff>
--- a/docs/source/_resources/tables/1_overview_benchmarks.xlsx
+++ b/docs/source/_resources/tables/1_overview_benchmarks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t xml:space="preserve">Level</t>
   </si>
@@ -203,6 +203,30 @@
   </si>
   <si>
     <t xml:space="preserve">1 (tail protein), 0 (non-tail protein)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOM_GSEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prediction of gamma-secretase substrates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breimann23c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (substrate), 0 (non-substrate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOM_GSEC_PU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prediction of gamma-secretase substrates (PU dataset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (substrate), 2 (unknown substrate status)</t>
   </si>
 </sst>
 </file>
@@ -323,15 +347,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K19:K20"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.77"/>
   </cols>
   <sheetData>
@@ -684,7 +708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -716,7 +740,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -748,6 +772,72 @@
         <v>60</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>92964</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>694</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>494524</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>